<commit_message>
working on data frame
</commit_message>
<xml_diff>
--- a/Wetlands/Wetlands_Baro_complete.xlsx
+++ b/Wetlands/Wetlands_Baro_complete.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\OneDrive\Documents\independent_research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kriddie/Documents/Ecuador2022/Wetlands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{35408B25-5A60-4BB0-A080-8A9EA6F34C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0170916B-91E7-134B-B811-191644E1772A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3897A001-682F-4FB9-A8FF-38EF11F16C6F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10300" xr2:uid="{3897A001-682F-4FB9-A8FF-38EF11F16C6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +85,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Sans"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -107,25 +113,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,27 +441,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDCCD1E6-90FA-413E-9366-EC817EAA5ED0}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.81640625" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
-    <col min="4" max="4" width="12.1796875" customWidth="1"/>
-    <col min="5" max="5" width="14.36328125" customWidth="1"/>
-    <col min="6" max="6" width="11.81640625" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -483,7 +484,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -503,7 +504,7 @@
         <v>3.662639</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -523,7 +524,7 @@
         <v>10.881159999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -543,27 +544,27 @@
         <v>15.192259999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="1">
         <v>44749</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="2">
         <v>0.50486111111111109</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="2">
         <v>0.53125</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6">
         <v>61.709899999999998</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6">
         <v>8.4652560000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2</v>
       </c>
@@ -583,7 +584,7 @@
         <v>7.0142429999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
@@ -603,27 +604,27 @@
         <v>17.12641</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>3</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="1">
         <v>44749</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="2">
         <v>0.53888888888888886</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="2">
         <v>0.56666666666666665</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9">
         <v>61.669130000000003</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9">
         <v>11.886049999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3</v>
       </c>
@@ -643,7 +644,7 @@
         <v>9.8485410000000009</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3</v>
       </c>
@@ -663,27 +664,27 @@
         <v>11.201510000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="6">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>4</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="1">
         <v>44741</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="2">
         <v>0.40625</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="2">
         <v>0.43055555555555558</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12">
         <v>62.187530000000002</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12">
         <v>5.3432000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>4</v>
       </c>
@@ -703,7 +704,7 @@
         <v>20.84094</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>4</v>
       </c>
@@ -723,7 +724,7 @@
         <v>8.4494000000000007</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>5</v>
       </c>
@@ -743,7 +744,7 @@
         <v>19.50581</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>5</v>
       </c>
@@ -753,7 +754,7 @@
       <c r="C16" s="2">
         <v>0.42499999999999999</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="2">
         <v>0.43541666666666662</v>
       </c>
       <c r="E16">
@@ -763,7 +764,7 @@
         <v>11.407019999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>5</v>
       </c>
@@ -783,28 +784,27 @@
         <v>9.1105940000000007</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
         <v>6</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="1">
         <v>44742</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="2">
         <v>0.3979166666666667</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="2">
         <v>0.4236111111111111</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="4">
         <v>62.315539999999999</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="3">
         <v>6.731376</v>
       </c>
-      <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>6</v>
       </c>
@@ -824,7 +824,7 @@
         <v>12.159700000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>6</v>
       </c>
@@ -844,28 +844,27 @@
         <v>8.528594</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="3" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="3">
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21">
         <v>7</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="1">
         <v>44742</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="2">
         <v>0.45208333333333334</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="2">
         <v>0.47847222222222219</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21">
         <v>62.579619999999998</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="5">
         <v>9.8802640000000004</v>
       </c>
-      <c r="G21" s="6"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>7</v>
       </c>
@@ -885,7 +884,7 @@
         <v>21.31306</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>7</v>
       </c>
@@ -905,7 +904,7 @@
         <v>10.54945</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>8</v>
       </c>
@@ -925,7 +924,7 @@
         <v>5.0080090000000004</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>8</v>
       </c>
@@ -945,7 +944,7 @@
         <v>7.9884050000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>8</v>
       </c>
@@ -965,7 +964,7 @@
         <v>8.6772130000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>9</v>
       </c>
@@ -975,7 +974,7 @@
       <c r="C27" s="2">
         <v>0.44236111111111115</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27" s="2">
         <v>0.46319444444444446</v>
       </c>
       <c r="E27">
@@ -985,7 +984,7 @@
         <v>5.3975980000000003</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>9</v>
       </c>
@@ -995,7 +994,7 @@
       <c r="C28" s="2">
         <v>0.39374999999999999</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="2">
         <v>0.4145833333333333</v>
       </c>
       <c r="E28">
@@ -1005,7 +1004,7 @@
         <v>11.34625</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>10</v>
       </c>
@@ -1025,7 +1024,7 @@
         <v>7.5037919999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>10</v>
       </c>
@@ -1045,7 +1044,7 @@
         <v>8.8268330000000006</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>10</v>
       </c>
@@ -1065,7 +1064,7 @@
         <v>9.4722810000000006</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>11</v>
       </c>
@@ -1075,7 +1074,7 @@
       <c r="C32" s="2">
         <v>0.45555555555555555</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="2">
         <v>0.47986111111111113</v>
       </c>
       <c r="E32">
@@ -1085,7 +1084,7 @@
         <v>14.99531</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>11</v>
       </c>
@@ -1095,7 +1094,7 @@
       <c r="C33" s="2">
         <v>0.45902777777777781</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D33" s="2">
         <v>0.47986111111111113</v>
       </c>
       <c r="E33">
@@ -1105,48 +1104,47 @@
         <v>10.485709999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34">
         <v>11</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B34" s="1">
         <v>44764</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34" s="2">
         <v>0.50138888888888888</v>
       </c>
-      <c r="D34" s="5">
+      <c r="D34" s="2">
         <v>0.52222222222222225</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34">
         <v>62.682319999999997</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34">
         <v>7.5193180000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35">
         <v>12</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35" s="1">
         <v>44748</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C35" s="2">
         <v>0.51666666666666672</v>
       </c>
-      <c r="D35" s="5">
+      <c r="D35" s="2">
         <v>0.54652777777777783</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E35">
         <v>62.709319999999998</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F35">
         <v>6.5932490000000001</v>
       </c>
-      <c r="G35" s="6"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>12</v>
       </c>
@@ -1166,7 +1164,7 @@
         <v>11.6134</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>12</v>
       </c>
@@ -1184,6 +1182,26 @@
       </c>
       <c r="F37">
         <v>8.6473669999999991</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>9</v>
+      </c>
+      <c r="B38" s="1">
+        <v>44750</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0.47847222222222219</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.48541666666666666</v>
+      </c>
+      <c r="E38" s="6">
+        <v>63.806420000000003</v>
+      </c>
+      <c r="F38" s="6">
+        <v>8.6296610000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>